<commit_message>
Mapping of all samples to co-assembly with megahit
</commit_message>
<xml_diff>
--- a/metadata/excel/projects/epfl/granular_sludge/metadata.xlsx
+++ b/metadata/excel/projects/epfl/granular_sludge/metadata.xlsx
@@ -9,17 +9,17 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="80" yWindow="460" windowWidth="48920" windowHeight="28240" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="28720" windowHeight="17540" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="micans_v6_ex1" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="150001" concurrentCalc="0"/>
   <customWorkbookViews>
+    <customWorkbookView name="Microsoft Office User - Personal View" guid="{31EA8456-A0B1-A842-BBBA-1FCBF1E560D2}" mergeInterval="0" personalView="1" maximized="1" windowWidth="2556" windowHeight="1244" tabRatio="500" activeSheetId="1"/>
+    <customWorkbookView name="Me - Personal View" guid="{22DA4066-82A0-D143-AA10-416CFBE3149D}" mergeInterval="0" personalView="1" xWindow="46" yWindow="23" windowWidth="1436" windowHeight="854" tabRatio="500" activeSheetId="1" showStatusbar="0"/>
+    <customWorkbookView name="Kemal - Personal View" guid="{CB40A2B6-4618-A74E-89AF-8E1F0A1F3C2E}" mergeInterval="0" personalView="1" xWindow="184" yWindow="84" windowWidth="1280" windowHeight="749" tabRatio="500" activeSheetId="1"/>
     <customWorkbookView name="LS - Personal View" guid="{06B92370-743D-804F-912C-658BE37B1274}" mergeInterval="0" personalView="1" maximized="1" windowWidth="2556" windowHeight="1244" tabRatio="500" activeSheetId="1"/>
-    <customWorkbookView name="Kemal - Personal View" guid="{CB40A2B6-4618-A74E-89AF-8E1F0A1F3C2E}" mergeInterval="0" personalView="1" xWindow="184" yWindow="84" windowWidth="1280" windowHeight="749" tabRatio="500" activeSheetId="1"/>
-    <customWorkbookView name="Me - Personal View" guid="{22DA4066-82A0-D143-AA10-416CFBE3149D}" mergeInterval="0" personalView="1" xWindow="46" yWindow="23" windowWidth="1436" windowHeight="854" tabRatio="500" activeSheetId="1" showStatusbar="0"/>
-    <customWorkbookView name="Microsoft Office User - Personal View" guid="{31EA8456-A0B1-A842-BBBA-1FCBF1E560D2}" mergeInterval="0" personalView="1" maximized="1" windowWidth="2556" windowHeight="1244" tabRatio="500" activeSheetId="1"/>
   </customWorkbookViews>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
@@ -4388,10 +4388,10 @@
   </sheetPr>
   <dimension ref="A1:BQ147"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="107" zoomScaleNormal="107" zoomScalePageLayoutView="107" workbookViewId="0">
-      <pane ySplit="2" topLeftCell="A105" activePane="bottomLeft" state="frozenSplit"/>
+    <sheetView tabSelected="1" topLeftCell="BB1" zoomScale="107" zoomScaleNormal="107" zoomScalePageLayoutView="107" workbookViewId="0">
+      <pane ySplit="2" topLeftCell="A4" activePane="bottomLeft" state="frozenSplit"/>
       <selection activeCell="X1" sqref="X1"/>
-      <selection pane="bottomLeft" activeCell="N68" sqref="N68"/>
+      <selection pane="bottomLeft" activeCell="BJ7" sqref="BJ7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -23932,19 +23932,9 @@
     <row r="147" spans="1:68" ht="17" thickTop="1" x14ac:dyDescent="0.2"/>
   </sheetData>
   <customSheetViews>
-    <customSheetView guid="{06B92370-743D-804F-912C-658BE37B1274}" topLeftCell="X1">
-      <pane ySplit="2" topLeftCell="A314" activePane="bottomLeft" state="frozenSplit"/>
-      <selection pane="bottomLeft" activeCell="AD344" sqref="AD344"/>
-      <rowBreaks count="2" manualBreakCount="2">
-        <brk id="1" max="16383" man="1"/>
-        <brk id="325" max="16383" man="1"/>
-      </rowBreaks>
-      <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-      <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
-    </customSheetView>
-    <customSheetView guid="{CB40A2B6-4618-A74E-89AF-8E1F0A1F3C2E}" topLeftCell="AP1">
-      <pane ySplit="2.03125" topLeftCell="A342" activePane="bottomLeft" state="frozenSplit"/>
-      <selection pane="bottomLeft" activeCell="BA367" sqref="BA367"/>
+    <customSheetView guid="{31EA8456-A0B1-A842-BBBA-1FCBF1E560D2}" topLeftCell="BD1">
+      <pane ySplit="2" topLeftCell="A273" activePane="bottomLeft" state="frozenSplit"/>
+      <selection pane="bottomLeft" activeCell="BG334" sqref="BG334"/>
       <rowBreaks count="2" manualBreakCount="2">
         <brk id="1" max="16383" man="1"/>
         <brk id="325" max="16383" man="1"/>
@@ -23962,14 +23952,24 @@
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
       <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
     </customSheetView>
-    <customSheetView guid="{31EA8456-A0B1-A842-BBBA-1FCBF1E560D2}" topLeftCell="BD1">
-      <pane ySplit="2" topLeftCell="A273" activePane="bottomLeft" state="frozenSplit"/>
-      <selection pane="bottomLeft" activeCell="BG334" sqref="BG334"/>
+    <customSheetView guid="{CB40A2B6-4618-A74E-89AF-8E1F0A1F3C2E}" topLeftCell="AP1">
+      <pane ySplit="2.03125" topLeftCell="A342" activePane="bottomLeft" state="frozenSplit"/>
+      <selection pane="bottomLeft" activeCell="BA367" sqref="BA367"/>
       <rowBreaks count="2" manualBreakCount="2">
         <brk id="1" max="16383" man="1"/>
         <brk id="325" max="16383" man="1"/>
       </rowBreaks>
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+      <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
+    </customSheetView>
+    <customSheetView guid="{06B92370-743D-804F-912C-658BE37B1274}" topLeftCell="X1">
+      <pane ySplit="2" topLeftCell="A314" activePane="bottomLeft" state="frozenSplit"/>
+      <selection pane="bottomLeft" activeCell="AD344" sqref="AD344"/>
+      <rowBreaks count="2" manualBreakCount="2">
+        <brk id="1" max="16383" man="1"/>
+        <brk id="325" max="16383" man="1"/>
+      </rowBreaks>
+      <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
       <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
     </customSheetView>
   </customSheetViews>

</xml_diff>